<commit_message>
Updated Sprint Backlog with recommended changes
</commit_message>
<xml_diff>
--- a/External/Documentation/sprint-1-backlog.xlsx
+++ b/External/Documentation/sprint-1-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomatech\Documents\Github\Cooktastrophe\External\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DACE694A-7C36-493F-97FA-62E3213E98F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DB079C-3C2D-4D72-BF97-93C4D8E30343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Project Management Templates</t>
   </si>
@@ -149,9 +149,6 @@
     <t>SPRINT 1 BACKLOG</t>
   </si>
   <si>
-    <t>As a developer I want to be able to test the game in a 2d format</t>
-  </si>
-  <si>
     <t>Create locomotion components bound to mouse and keyboard inputs</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>US005</t>
   </si>
   <si>
-    <t>As a player I want to be able to cook customers orders</t>
-  </si>
-  <si>
     <t>Implement a system to list all types of food and create recipes to turn one or more types of food into another type of food</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>US011</t>
   </si>
   <si>
-    <t>As a player I want to be able to move around.</t>
-  </si>
-  <si>
     <t>Install and setup Unity's VR Interaction Toolkit package</t>
   </si>
   <si>
@@ -195,6 +186,18 @@
   </si>
   <si>
     <t xml:space="preserve">Implement a way for vertical camera rotation to be registered by the mouse </t>
+  </si>
+  <si>
+    <t>As a developer I want to be able to test the game in a 2d format. Acceptance Criteria: Testing Completed</t>
+  </si>
+  <si>
+    <t>As a player I want to be able to cook customers orders. Acceptance Criteria: Testing Completed</t>
+  </si>
+  <si>
+    <t>As a player I want to be able to move around. Acceptance Criteria: Testing Completed</t>
+  </si>
+  <si>
+    <t>Test functionality</t>
   </si>
 </sst>
 </file>
@@ -281,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -545,12 +548,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -636,50 +665,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1079,10 +1120,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="B6:AC24"/>
+  <dimension ref="B6:AC27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,29 +1139,29 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:29" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36"/>
-      <c r="U6" s="36"/>
-      <c r="V6" s="37"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="34"/>
     </row>
     <row r="7" spans="2:29" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:29" s="10" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1199,11 +1240,11 @@
       <c r="B9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>35</v>
@@ -1211,7 +1252,7 @@
       <c r="F9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="35">
         <v>20</v>
       </c>
       <c r="H9" s="18">
@@ -1262,9 +1303,9 @@
     </row>
     <row r="10" spans="2:29" s="8" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="39"/>
-      <c r="C10" s="33"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>35</v>
@@ -1272,7 +1313,7 @@
       <c r="F10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="33"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="7">
         <v>0</v>
       </c>
@@ -1319,581 +1360,689 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:29" s="8" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="24" t="s">
+    <row r="11" spans="2:29" s="8" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="39"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="44">
+        <v>0</v>
+      </c>
+      <c r="I11" s="44">
+        <v>0</v>
+      </c>
+      <c r="J11" s="44">
+        <v>6</v>
+      </c>
+      <c r="K11" s="44">
+        <v>0</v>
+      </c>
+      <c r="L11" s="44">
+        <v>0</v>
+      </c>
+      <c r="M11" s="44">
+        <v>0</v>
+      </c>
+      <c r="N11" s="44">
+        <v>0</v>
+      </c>
+      <c r="O11" s="44">
+        <v>0</v>
+      </c>
+      <c r="P11" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="44">
+        <v>0</v>
+      </c>
+      <c r="R11" s="44">
+        <v>0</v>
+      </c>
+      <c r="S11" s="44">
+        <v>0</v>
+      </c>
+      <c r="T11" s="44">
+        <v>0</v>
+      </c>
+      <c r="U11" s="44">
+        <v>0</v>
+      </c>
+      <c r="V11" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:29" s="8" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="40"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="37"/>
+      <c r="H12" s="21">
+        <v>0</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0</v>
+      </c>
+      <c r="J12" s="21">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0</v>
+      </c>
+      <c r="L12" s="21">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0</v>
+      </c>
+      <c r="N12" s="21">
+        <v>0</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0</v>
+      </c>
+      <c r="P12" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>0</v>
+      </c>
+      <c r="R12" s="21">
+        <v>0</v>
+      </c>
+      <c r="S12" s="21">
+        <v>0</v>
+      </c>
+      <c r="T12" s="21">
+        <v>0</v>
+      </c>
+      <c r="U12" s="21">
+        <v>0</v>
+      </c>
+      <c r="V12" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:29" s="8" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="21">
-        <v>0</v>
-      </c>
-      <c r="I11" s="21">
-        <v>0</v>
-      </c>
-      <c r="J11" s="21">
-        <v>6</v>
-      </c>
-      <c r="K11" s="21">
-        <v>2</v>
-      </c>
-      <c r="L11" s="21">
-        <v>0</v>
-      </c>
-      <c r="M11" s="21">
-        <v>0</v>
-      </c>
-      <c r="N11" s="21">
-        <v>0</v>
-      </c>
-      <c r="O11" s="21">
-        <v>0</v>
-      </c>
-      <c r="P11" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="21">
-        <v>0</v>
-      </c>
-      <c r="R11" s="21">
-        <v>0</v>
-      </c>
-      <c r="S11" s="21">
-        <v>0</v>
-      </c>
-      <c r="T11" s="21">
-        <v>0</v>
-      </c>
-      <c r="U11" s="21">
-        <v>0</v>
-      </c>
-      <c r="V11" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:29" s="8" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
+      <c r="C13" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="29">
-        <v>48</v>
-      </c>
-      <c r="H12" s="18">
-        <v>0</v>
-      </c>
-      <c r="I12" s="18">
-        <v>0</v>
-      </c>
-      <c r="J12" s="18">
-        <v>5</v>
-      </c>
-      <c r="K12" s="18">
-        <v>7</v>
-      </c>
-      <c r="L12" s="18">
-        <v>2</v>
-      </c>
-      <c r="M12" s="18">
-        <v>8</v>
-      </c>
-      <c r="N12" s="18">
-        <v>6</v>
-      </c>
-      <c r="O12" s="18">
-        <v>6</v>
-      </c>
-      <c r="P12" s="18">
-        <v>5</v>
-      </c>
-      <c r="Q12" s="18">
-        <v>0</v>
-      </c>
-      <c r="R12" s="18">
-        <v>0</v>
-      </c>
-      <c r="S12" s="18">
-        <v>0</v>
-      </c>
-      <c r="T12" s="18">
-        <v>0</v>
-      </c>
-      <c r="U12" s="18">
-        <v>0</v>
-      </c>
-      <c r="V12" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:29" s="8" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="42">
-        <v>0</v>
-      </c>
-      <c r="I13" s="42">
-        <v>0</v>
-      </c>
-      <c r="J13" s="42">
-        <v>0</v>
-      </c>
-      <c r="K13" s="42">
-        <v>0</v>
-      </c>
-      <c r="L13" s="42">
-        <v>0</v>
-      </c>
-      <c r="M13" s="42">
-        <v>0</v>
-      </c>
-      <c r="N13" s="42">
-        <v>0</v>
-      </c>
-      <c r="O13" s="42">
-        <v>0</v>
-      </c>
-      <c r="P13" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="42">
-        <v>0</v>
-      </c>
-      <c r="R13" s="42">
-        <v>0</v>
-      </c>
-      <c r="S13" s="42">
-        <v>0</v>
-      </c>
-      <c r="T13" s="42">
-        <v>0</v>
-      </c>
-      <c r="U13" s="42">
-        <v>0</v>
-      </c>
-      <c r="V13" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:29" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="32"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="42" t="s">
+      <c r="F13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="35">
+        <v>48</v>
+      </c>
+      <c r="H13" s="18">
+        <v>0</v>
+      </c>
+      <c r="I13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J13" s="18">
+        <v>5</v>
+      </c>
+      <c r="K13" s="18">
+        <v>7</v>
+      </c>
+      <c r="L13" s="18">
+        <v>2</v>
+      </c>
+      <c r="M13" s="18">
+        <v>8</v>
+      </c>
+      <c r="N13" s="18">
+        <v>6</v>
+      </c>
+      <c r="O13" s="18">
+        <v>6</v>
+      </c>
+      <c r="P13" s="18">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="18">
+        <v>0</v>
+      </c>
+      <c r="R13" s="18">
+        <v>0</v>
+      </c>
+      <c r="S13" s="18">
+        <v>0</v>
+      </c>
+      <c r="T13" s="18">
+        <v>0</v>
+      </c>
+      <c r="U13" s="18">
+        <v>0</v>
+      </c>
+      <c r="V13" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:29" s="8" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="42"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="21">
-        <v>0</v>
-      </c>
-      <c r="I14" s="21">
-        <v>0</v>
-      </c>
-      <c r="J14" s="21">
-        <v>0</v>
-      </c>
-      <c r="K14" s="21">
-        <v>0</v>
-      </c>
-      <c r="L14" s="21">
-        <v>0</v>
-      </c>
-      <c r="M14" s="21">
-        <v>0</v>
-      </c>
-      <c r="N14" s="21">
-        <v>0</v>
-      </c>
-      <c r="O14" s="21">
-        <v>0</v>
-      </c>
-      <c r="P14" s="21">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="21">
-        <v>3</v>
-      </c>
-      <c r="R14" s="21">
-        <v>0</v>
-      </c>
-      <c r="S14" s="21">
-        <v>0</v>
-      </c>
-      <c r="T14" s="21">
-        <v>0</v>
-      </c>
-      <c r="U14" s="21">
-        <v>0</v>
-      </c>
-      <c r="V14" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:29" s="8" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>49</v>
+      <c r="F14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="30">
+        <v>0</v>
+      </c>
+      <c r="I14" s="30">
+        <v>0</v>
+      </c>
+      <c r="J14" s="30">
+        <v>0</v>
+      </c>
+      <c r="K14" s="30">
+        <v>0</v>
+      </c>
+      <c r="L14" s="30">
+        <v>0</v>
+      </c>
+      <c r="M14" s="30">
+        <v>0</v>
+      </c>
+      <c r="N14" s="30">
+        <v>0</v>
+      </c>
+      <c r="O14" s="30">
+        <v>0</v>
+      </c>
+      <c r="P14" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="30">
+        <v>0</v>
+      </c>
+      <c r="R14" s="30">
+        <v>0</v>
+      </c>
+      <c r="S14" s="30">
+        <v>0</v>
+      </c>
+      <c r="T14" s="30">
+        <v>0</v>
+      </c>
+      <c r="U14" s="30">
+        <v>0</v>
+      </c>
+      <c r="V14" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:29" s="8" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="42"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="29">
-        <v>10</v>
-      </c>
-      <c r="H15" s="18">
-        <v>0</v>
-      </c>
-      <c r="I15" s="18">
-        <v>0</v>
-      </c>
-      <c r="J15" s="18">
-        <v>0</v>
-      </c>
-      <c r="K15" s="18">
-        <v>0</v>
-      </c>
-      <c r="L15" s="18">
-        <v>0</v>
-      </c>
-      <c r="M15" s="18">
-        <v>0</v>
-      </c>
-      <c r="N15" s="18">
-        <v>0</v>
-      </c>
-      <c r="O15" s="18">
-        <v>0</v>
-      </c>
-      <c r="P15" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="18">
-        <v>0</v>
-      </c>
-      <c r="R15" s="18">
+      <c r="G15" s="36"/>
+      <c r="H15" s="44">
+        <v>0</v>
+      </c>
+      <c r="I15" s="44">
+        <v>0</v>
+      </c>
+      <c r="J15" s="44">
+        <v>0</v>
+      </c>
+      <c r="K15" s="44">
+        <v>0</v>
+      </c>
+      <c r="L15" s="44">
+        <v>0</v>
+      </c>
+      <c r="M15" s="44">
+        <v>0</v>
+      </c>
+      <c r="N15" s="44">
+        <v>0</v>
+      </c>
+      <c r="O15" s="44">
+        <v>0</v>
+      </c>
+      <c r="P15" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="44">
+        <v>0</v>
+      </c>
+      <c r="R15" s="44">
+        <v>0</v>
+      </c>
+      <c r="S15" s="44">
+        <v>0</v>
+      </c>
+      <c r="T15" s="44">
+        <v>0</v>
+      </c>
+      <c r="U15" s="44">
+        <v>0</v>
+      </c>
+      <c r="V15" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:29" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="43"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="37"/>
+      <c r="H16" s="21">
+        <v>0</v>
+      </c>
+      <c r="I16" s="21">
+        <v>0</v>
+      </c>
+      <c r="J16" s="21">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0</v>
+      </c>
+      <c r="L16" s="21">
+        <v>0</v>
+      </c>
+      <c r="M16" s="21">
+        <v>0</v>
+      </c>
+      <c r="N16" s="21">
+        <v>0</v>
+      </c>
+      <c r="O16" s="21">
+        <v>0</v>
+      </c>
+      <c r="P16" s="21">
         <v>2</v>
       </c>
-      <c r="S15" s="18">
-        <v>0</v>
-      </c>
-      <c r="T15" s="18">
-        <v>0</v>
-      </c>
-      <c r="U15" s="18">
-        <v>0</v>
-      </c>
-      <c r="V15" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:29" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="15">
-        <v>0</v>
-      </c>
-      <c r="I16" s="15">
-        <v>0</v>
-      </c>
-      <c r="J16" s="15">
-        <v>0</v>
-      </c>
-      <c r="K16" s="15">
-        <v>0</v>
-      </c>
-      <c r="L16" s="15">
-        <v>0</v>
-      </c>
-      <c r="M16" s="15">
-        <v>0</v>
-      </c>
-      <c r="N16" s="15">
-        <v>0</v>
-      </c>
-      <c r="O16" s="15">
-        <v>0</v>
-      </c>
-      <c r="P16" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="15">
-        <v>0</v>
-      </c>
-      <c r="R16" s="15">
-        <v>0</v>
-      </c>
-      <c r="S16" s="15">
-        <v>8</v>
-      </c>
-      <c r="T16" s="15">
-        <v>6</v>
-      </c>
-      <c r="U16" s="15">
-        <v>0</v>
-      </c>
-      <c r="V16" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="7" t="s">
-        <v>52</v>
+      <c r="Q16" s="21">
+        <v>3</v>
+      </c>
+      <c r="R16" s="21">
+        <v>0</v>
+      </c>
+      <c r="S16" s="21">
+        <v>0</v>
+      </c>
+      <c r="T16" s="21">
+        <v>0</v>
+      </c>
+      <c r="U16" s="21">
+        <v>0</v>
+      </c>
+      <c r="V16" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" s="8" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="15">
-        <v>0</v>
-      </c>
-      <c r="I17" s="15">
-        <v>0</v>
-      </c>
-      <c r="J17" s="15">
-        <v>0</v>
-      </c>
-      <c r="K17" s="15">
-        <v>0</v>
-      </c>
-      <c r="L17" s="15">
-        <v>0</v>
-      </c>
-      <c r="M17" s="15">
-        <v>0</v>
-      </c>
-      <c r="N17" s="15">
-        <v>0</v>
-      </c>
-      <c r="O17" s="15">
-        <v>0</v>
-      </c>
-      <c r="P17" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="15">
-        <v>0</v>
-      </c>
-      <c r="R17" s="15">
-        <v>0</v>
-      </c>
-      <c r="S17" s="15">
-        <v>0</v>
-      </c>
-      <c r="T17" s="15">
-        <v>0</v>
-      </c>
-      <c r="U17" s="15">
+      <c r="G17" s="35">
+        <v>10</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0</v>
+      </c>
+      <c r="I17" s="18">
+        <v>0</v>
+      </c>
+      <c r="J17" s="18">
+        <v>0</v>
+      </c>
+      <c r="K17" s="18">
+        <v>0</v>
+      </c>
+      <c r="L17" s="18">
+        <v>0</v>
+      </c>
+      <c r="M17" s="18">
+        <v>0</v>
+      </c>
+      <c r="N17" s="18">
+        <v>0</v>
+      </c>
+      <c r="O17" s="18">
+        <v>0</v>
+      </c>
+      <c r="P17" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>0</v>
+      </c>
+      <c r="R17" s="18">
+        <v>2</v>
+      </c>
+      <c r="S17" s="18">
+        <v>0</v>
+      </c>
+      <c r="T17" s="18">
+        <v>0</v>
+      </c>
+      <c r="U17" s="18">
+        <v>0</v>
+      </c>
+      <c r="V17" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="42"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="15">
+        <v>0</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0</v>
+      </c>
+      <c r="K18" s="15">
+        <v>0</v>
+      </c>
+      <c r="L18" s="15">
+        <v>0</v>
+      </c>
+      <c r="M18" s="15">
+        <v>0</v>
+      </c>
+      <c r="N18" s="15">
+        <v>0</v>
+      </c>
+      <c r="O18" s="15">
+        <v>0</v>
+      </c>
+      <c r="P18" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="15">
+        <v>0</v>
+      </c>
+      <c r="R18" s="15">
+        <v>0</v>
+      </c>
+      <c r="S18" s="15">
+        <v>8</v>
+      </c>
+      <c r="T18" s="15">
+        <v>6</v>
+      </c>
+      <c r="U18" s="15">
+        <v>0</v>
+      </c>
+      <c r="V18" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="42"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="15">
+        <v>0</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15">
+        <v>0</v>
+      </c>
+      <c r="K19" s="15">
+        <v>0</v>
+      </c>
+      <c r="L19" s="15">
+        <v>0</v>
+      </c>
+      <c r="M19" s="15">
+        <v>0</v>
+      </c>
+      <c r="N19" s="15">
+        <v>0</v>
+      </c>
+      <c r="O19" s="15">
+        <v>0</v>
+      </c>
+      <c r="P19" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="15">
+        <v>0</v>
+      </c>
+      <c r="R19" s="15">
+        <v>0</v>
+      </c>
+      <c r="S19" s="15">
+        <v>0</v>
+      </c>
+      <c r="T19" s="15">
+        <v>0</v>
+      </c>
+      <c r="U19" s="15">
         <v>4</v>
       </c>
-      <c r="V17" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:22" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="32"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="24" t="s">
+      <c r="V19" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="42"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="22">
-        <v>0</v>
-      </c>
-      <c r="I18" s="22">
-        <v>0</v>
-      </c>
-      <c r="J18" s="22">
-        <v>0</v>
-      </c>
-      <c r="K18" s="22">
-        <v>0</v>
-      </c>
-      <c r="L18" s="22">
-        <v>0</v>
-      </c>
-      <c r="M18" s="22">
-        <v>0</v>
-      </c>
-      <c r="N18" s="22">
-        <v>0</v>
-      </c>
-      <c r="O18" s="22">
-        <v>0</v>
-      </c>
-      <c r="P18" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="22">
-        <v>0</v>
-      </c>
-      <c r="R18" s="22">
-        <v>0</v>
-      </c>
-      <c r="S18" s="22">
-        <v>0</v>
-      </c>
-      <c r="T18" s="22">
-        <v>0</v>
-      </c>
-      <c r="U18" s="22">
-        <v>0</v>
-      </c>
-      <c r="V18" s="23">
+      <c r="G20" s="36"/>
+      <c r="H20" s="46">
+        <v>0</v>
+      </c>
+      <c r="I20" s="46">
+        <v>0</v>
+      </c>
+      <c r="J20" s="46">
+        <v>0</v>
+      </c>
+      <c r="K20" s="46">
+        <v>0</v>
+      </c>
+      <c r="L20" s="46">
+        <v>0</v>
+      </c>
+      <c r="M20" s="46">
+        <v>0</v>
+      </c>
+      <c r="N20" s="46">
+        <v>0</v>
+      </c>
+      <c r="O20" s="46">
+        <v>0</v>
+      </c>
+      <c r="P20" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="46">
+        <v>0</v>
+      </c>
+      <c r="R20" s="46">
+        <v>0</v>
+      </c>
+      <c r="S20" s="46">
+        <v>0</v>
+      </c>
+      <c r="T20" s="46">
+        <v>0</v>
+      </c>
+      <c r="U20" s="46">
+        <v>0</v>
+      </c>
+      <c r="V20" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="43"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="37"/>
+      <c r="H21" s="22">
+        <v>0</v>
+      </c>
+      <c r="I21" s="22">
+        <v>0</v>
+      </c>
+      <c r="J21" s="22">
+        <v>0</v>
+      </c>
+      <c r="K21" s="22">
+        <v>0</v>
+      </c>
+      <c r="L21" s="22">
+        <v>0</v>
+      </c>
+      <c r="M21" s="22">
+        <v>0</v>
+      </c>
+      <c r="N21" s="22">
+        <v>0</v>
+      </c>
+      <c r="O21" s="22">
+        <v>0</v>
+      </c>
+      <c r="P21" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="22">
+        <v>0</v>
+      </c>
+      <c r="R21" s="22">
+        <v>0</v>
+      </c>
+      <c r="S21" s="22">
+        <v>0</v>
+      </c>
+      <c r="T21" s="22">
+        <v>0</v>
+      </c>
+      <c r="U21" s="22">
+        <v>0</v>
+      </c>
+      <c r="V21" s="23">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="17"/>
-      <c r="V19" s="17"/>
-    </row>
-    <row r="20" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-    </row>
-    <row r="21" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-    </row>
     <row r="22" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
     </row>
     <row r="23" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
@@ -1924,83 +2073,152 @@
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="16">
-        <f>SUM(G9:G23)</f>
+      <c r="G24" s="6"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+    </row>
+    <row r="25" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+    </row>
+    <row r="26" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+    </row>
+    <row r="27" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="16">
+        <f t="shared" ref="G27:V27" si="0">SUM(G9:G26)</f>
         <v>78</v>
       </c>
-      <c r="H24" s="16">
-        <f>SUM(H9:H23)</f>
+      <c r="H27" s="16">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="I24" s="16">
-        <f>SUM(I9:I23)</f>
+      <c r="I27" s="16">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J24" s="16">
-        <f>SUM(J9:J23)</f>
+      <c r="J27" s="16">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="K24" s="16">
-        <f>SUM(K9:K23)</f>
-        <v>9</v>
-      </c>
-      <c r="L24" s="16">
-        <f>SUM(L9:L23)</f>
+      <c r="K27" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L27" s="16">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M24" s="16">
-        <f>SUM(M9:M23)</f>
+      <c r="M27" s="16">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="N24" s="16">
-        <f>SUM(N9:N23)</f>
+      <c r="N27" s="16">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="O24" s="16">
-        <f>SUM(O9:O23)</f>
+      <c r="O27" s="16">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="P24" s="16">
-        <f>SUM(P9:P23)</f>
+      <c r="P27" s="16">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q24" s="16">
-        <f>SUM(Q9:Q23)</f>
+      <c r="Q27" s="16">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R24" s="16">
-        <f>SUM(R9:R23)</f>
+      <c r="R27" s="16">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="S24" s="16">
-        <f>SUM(S9:S23)</f>
+      <c r="S27" s="16">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="T24" s="16">
-        <f>SUM(T9:T23)</f>
+      <c r="T27" s="16">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="U24" s="16">
-        <f>SUM(U9:U23)</f>
+      <c r="U27" s="16">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="V24" s="16">
-        <f>SUM(V9:V23)</f>
+      <c r="V27" s="16">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="G17:G21"/>
     <mergeCell ref="B6:V6"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B13:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2053,7 +2271,7 @@
       <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="29">
         <v>45035</v>
       </c>
     </row>

</xml_diff>